<commit_message>
Fase 2 - Final - fecha 22-11-24 (previo termino)
está todo, falta el código fuente, apk, y video
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de documentación/Listado de CU y Listado de RF y RNF/Lista de requerimientos funcionales y no funcionales.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de documentación/Listado de CU y Listado de RF y RNF/Lista de requerimientos funcionales y no funcionales.xlsx
@@ -736,7 +736,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,6 +771,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -923,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -960,6 +966,9 @@
     <xf borderId="4" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -984,19 +993,19 @@
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1794,8 +1803,8 @@
       <c r="H12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>53</v>
+      <c r="I12" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
@@ -2041,7 +2050,7 @@
       <c r="K17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="L17" s="12"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -2176,7 +2185,7 @@
         <v>17</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="14" t="s">
         <v>96</v>
       </c>
       <c r="J20" s="8"/>
@@ -2200,33 +2209,33 @@
       <c r="Z20" s="11"/>
     </row>
     <row r="21" ht="57.75" customHeight="1">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="16" t="s">
         <v>100</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="16"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="15" t="s">
+      <c r="J21" s="18"/>
+      <c r="K21" s="16" t="s">
         <v>101</v>
       </c>
       <c r="L21" s="3"/>
@@ -2267,11 +2276,11 @@
       <c r="G22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="18"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="20"/>
       <c r="K22" s="5" t="s">
         <v>105</v>
       </c>
@@ -2313,11 +2322,11 @@
       <c r="G23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="18"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="21" t="s">
         <v>109</v>
       </c>
       <c r="K23" s="5" t="s">
@@ -2340,7 +2349,7 @@
       <c r="Z23" s="11"/>
     </row>
     <row r="24" ht="101.25" customHeight="1">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="15" t="s">
         <v>111</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -2361,11 +2370,11 @@
       <c r="G24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="18"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J24" s="21"/>
+      <c r="J24" s="22"/>
       <c r="K24" s="5" t="s">
         <v>114</v>
       </c>
@@ -2386,7 +2395,7 @@
       <c r="Z24" s="11"/>
     </row>
     <row r="25" ht="101.25" customHeight="1">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>115</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -2407,11 +2416,11 @@
       <c r="G25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="18"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J25" s="21"/>
+      <c r="J25" s="22"/>
       <c r="K25" s="5" t="s">
         <v>118</v>
       </c>
@@ -2432,7 +2441,7 @@
       <c r="Z25" s="11"/>
     </row>
     <row r="26" ht="101.25" customHeight="1">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="15" t="s">
         <v>119</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -2453,11 +2462,11 @@
       <c r="G26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="18"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J26" s="21"/>
+      <c r="J26" s="22"/>
       <c r="K26" s="5" t="s">
         <v>122</v>
       </c>
@@ -2478,7 +2487,7 @@
       <c r="Z26" s="11"/>
     </row>
     <row r="27" ht="101.25" customHeight="1">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="15" t="s">
         <v>123</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -2499,11 +2508,11 @@
       <c r="G27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="18"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J27" s="21"/>
+      <c r="J27" s="22"/>
       <c r="K27" s="5" t="s">
         <v>126</v>
       </c>
@@ -2524,13 +2533,13 @@
       <c r="Z27" s="11"/>
     </row>
     <row r="28" ht="101.25" customHeight="1">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="15" t="s">
         <v>127</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>128</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -2545,11 +2554,11 @@
       <c r="G28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="18"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J28" s="21"/>
+      <c r="J28" s="22"/>
       <c r="K28" s="5" t="s">
         <v>130</v>
       </c>
@@ -2570,16 +2579,16 @@
       <c r="Z28" s="11"/>
     </row>
     <row r="29" ht="101.25" customHeight="1">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E29" s="6" t="s">
@@ -2591,11 +2600,11 @@
       <c r="G29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="18"/>
+      <c r="H29" s="19"/>
       <c r="I29" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J29" s="21"/>
+      <c r="J29" s="22"/>
       <c r="K29" s="5" t="s">
         <v>134</v>
       </c>
@@ -2616,16 +2625,16 @@
       <c r="Z29" s="11"/>
     </row>
     <row r="30" ht="101.25" customHeight="1">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="20" t="s">
         <v>137</v>
       </c>
       <c r="E30" s="6" t="s">
@@ -2637,11 +2646,11 @@
       <c r="G30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="18"/>
+      <c r="H30" s="19"/>
       <c r="I30" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="J30" s="21"/>
+      <c r="J30" s="22"/>
       <c r="K30" s="5" t="s">
         <v>138</v>
       </c>
@@ -2662,7 +2671,7 @@
       <c r="Z30" s="11"/>
     </row>
     <row r="31" ht="60.75" customHeight="1">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="15" t="s">
         <v>139</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -2674,7 +2683,7 @@
       <c r="D31" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -2720,7 +2729,7 @@
       <c r="D32" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -2766,7 +2775,7 @@
       <c r="D33" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F33" s="5" t="s">
@@ -2800,7 +2809,7 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34" ht="61.5" customHeight="1">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="15" t="s">
         <v>152</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -2812,7 +2821,7 @@
       <c r="D34" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -2858,7 +2867,7 @@
       <c r="D35" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E35" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -2904,7 +2913,7 @@
       <c r="D36" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -2938,7 +2947,7 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="15" t="s">
         <v>164</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -2950,7 +2959,7 @@
       <c r="D37" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -2996,7 +3005,7 @@
       <c r="D38" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E38" s="22" t="s">
+      <c r="E38" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -3042,7 +3051,7 @@
       <c r="D39" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -3076,7 +3085,7 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="15" t="s">
         <v>177</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -3088,7 +3097,7 @@
       <c r="D40" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -3134,7 +3143,7 @@
       <c r="D41" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F41" s="5" t="s">
@@ -3180,7 +3189,7 @@
       <c r="D42" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F42" s="5" t="s">
@@ -3214,7 +3223,7 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="15" t="s">
         <v>189</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -3226,7 +3235,7 @@
       <c r="D43" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F43" s="5" t="s">
@@ -3263,30 +3272,30 @@
       <c r="A44" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="E44" s="23" t="s">
+      <c r="E44" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G44" s="15" t="s">
+      <c r="G44" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="15"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15" t="s">
+      <c r="J44" s="16"/>
+      <c r="K44" s="16" t="s">
         <v>196</v>
       </c>
       <c r="L44" s="3"/>
@@ -3306,25 +3315,25 @@
       <c r="Z44" s="3"/>
     </row>
     <row r="45" ht="86.25" customHeight="1">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="19" t="s">
         <v>198</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G45" s="16" t="s">
         <v>17</v>
       </c>
       <c r="H45" s="5"/>
@@ -3355,7 +3364,7 @@
       <c r="A46" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -3364,13 +3373,13 @@
       <c r="D46" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E46" s="25" t="s">
         <v>142</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="15" t="s">
+      <c r="G46" s="16" t="s">
         <v>17</v>
       </c>
       <c r="H46" s="5"/>
@@ -3398,10 +3407,10 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" ht="68.25" customHeight="1">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="16" t="s">
         <v>165</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -3410,13 +3419,13 @@
       <c r="D47" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E47" s="22" t="s">
+      <c r="E47" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="G47" s="16" t="s">
         <v>17</v>
       </c>
       <c r="H47" s="5"/>
@@ -3447,7 +3456,7 @@
       <c r="A48" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -3456,13 +3465,13 @@
       <c r="D48" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="E48" s="22" t="s">
+      <c r="E48" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G48" s="16" t="s">
         <v>17</v>
       </c>
       <c r="H48" s="5"/>
@@ -3490,32 +3499,32 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="26" t="s">
         <v>214</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="E49" s="22" t="s">
+      <c r="E49" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="25"/>
+      <c r="H49" s="26"/>
       <c r="I49" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J49" s="25"/>
+      <c r="J49" s="26"/>
       <c r="K49" s="5" t="s">
         <v>216</v>
       </c>
@@ -3542,26 +3551,26 @@
       <c r="B50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="E50" s="22" t="s">
+      <c r="E50" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F50" s="26" t="s">
+      <c r="F50" s="27" t="s">
         <v>16</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H50" s="25"/>
+      <c r="H50" s="26"/>
       <c r="I50" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J50" s="25"/>
+      <c r="J50" s="26"/>
       <c r="K50" s="5" t="s">
         <v>212</v>
       </c>

</xml_diff>